<commit_message>
feat: calculate the expected return and std dev for each portfolio possible
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomasrolimmiele/Desktop/Portfolio-Modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B967939-823F-8E47-8356-DA8CB7BADD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9093F773-EE1B-144D-8F20-3BAC6199A984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17660" xr2:uid="{A4BAA6AD-8670-4447-B2CD-9AF3FDDAD6EB}"/>
   </bookViews>
@@ -100,7 +100,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,6 +157,20 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -365,7 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -436,9 +450,6 @@
     <xf numFmtId="10" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -511,6 +522,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,43 +870,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECA463D-541C-684E-B0C3-10ECCBC46BBC}">
-  <dimension ref="A6:KV60"/>
+  <dimension ref="A5:KV60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="6" spans="2:308" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:308" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:308" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="2:308" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:308" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="2:308" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:308" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="2:308" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:308" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="11" spans="2:308" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:308" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
         <v>4</v>
       </c>
@@ -1198,18 +1223,18 @@
       <c r="KU11" s="16"/>
       <c r="KV11" s="16"/>
     </row>
-    <row r="13" spans="2:308" x14ac:dyDescent="0.2">
-      <c r="B13" s="46" t="s">
+    <row r="13" spans="1:308" x14ac:dyDescent="0.2">
+      <c r="B13" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="48"/>
-    </row>
-    <row r="14" spans="2:308" x14ac:dyDescent="0.2">
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="47"/>
+    </row>
+    <row r="14" spans="1:308" x14ac:dyDescent="0.2">
       <c r="B14" s="13" t="s">
         <v>6</v>
       </c>
@@ -1228,7 +1253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:308" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:308" x14ac:dyDescent="0.2">
       <c r="B15" s="14" t="s">
         <v>7</v>
       </c>
@@ -1243,7 +1268,7 @@
       <c r="H15" s="20"/>
     </row>
     <row r="17" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -1555,7 +1580,7 @@
       <c r="KU17" s="21"/>
     </row>
     <row r="18" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="B18" s="50"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="11" t="s">
         <v>13</v>
       </c>
@@ -1867,20 +1892,20 @@
     <row r="21" spans="1:308" x14ac:dyDescent="0.2">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="46" t="s">
+      <c r="E21" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="48"/>
-    </row>
-    <row r="22" spans="1:308" x14ac:dyDescent="0.2">
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
+    </row>
+    <row r="22" spans="1:308" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>14</v>
       </c>
@@ -1889,9 +1914,9 @@
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="26"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
       <c r="H22" s="27"/>
       <c r="I22" s="27"/>
       <c r="J22" s="27"/>
@@ -2195,858 +2220,858 @@
       <c r="KV22" s="27"/>
     </row>
     <row r="23" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="A23" s="36">
+      <c r="A23" s="35">
         <v>-1</v>
       </c>
-      <c r="B23" s="37">
+      <c r="B23" s="36">
         <f>1-A23</f>
         <v>2</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="29"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="45"/>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="45"/>
-      <c r="S23" s="45"/>
-      <c r="T23" s="45"/>
-      <c r="U23" s="45"/>
-      <c r="V23" s="45"/>
-      <c r="W23" s="45"/>
-      <c r="X23" s="45"/>
-      <c r="Y23" s="45"/>
-      <c r="Z23" s="45"/>
-      <c r="AA23" s="45"/>
-      <c r="AB23" s="45"/>
-      <c r="AC23" s="45"/>
-      <c r="AD23" s="45"/>
-      <c r="AE23" s="45"/>
-      <c r="AF23" s="45"/>
-      <c r="AG23" s="45"/>
-      <c r="AH23" s="45"/>
-      <c r="AI23" s="45"/>
-      <c r="AJ23" s="45"/>
-      <c r="AK23" s="45"/>
-      <c r="AL23" s="45"/>
-      <c r="AM23" s="45"/>
-      <c r="AN23" s="45"/>
-      <c r="AO23" s="45"/>
-      <c r="AP23" s="45"/>
-      <c r="AQ23" s="45"/>
-      <c r="AR23" s="45"/>
-      <c r="AS23" s="45"/>
-      <c r="AT23" s="45"/>
-      <c r="AU23" s="45"/>
-      <c r="AV23" s="45"/>
-      <c r="AW23" s="45"/>
-      <c r="AX23" s="45"/>
-      <c r="AY23" s="45"/>
-      <c r="AZ23" s="45"/>
-      <c r="BA23" s="45"/>
-      <c r="BB23" s="45"/>
-      <c r="BC23" s="45"/>
-      <c r="BD23" s="45"/>
-      <c r="BE23" s="45"/>
-      <c r="BF23" s="45"/>
-      <c r="BG23" s="45"/>
-      <c r="BH23" s="45"/>
-      <c r="BI23" s="45"/>
-      <c r="BJ23" s="45"/>
-      <c r="BK23" s="45"/>
-      <c r="BL23" s="45"/>
-      <c r="BM23" s="45"/>
-      <c r="BN23" s="45"/>
-      <c r="BO23" s="45"/>
-      <c r="BP23" s="45"/>
-      <c r="BQ23" s="45"/>
-      <c r="BR23" s="45"/>
-      <c r="BS23" s="45"/>
-      <c r="BT23" s="45"/>
-      <c r="BU23" s="45"/>
-      <c r="BV23" s="45"/>
-      <c r="BW23" s="45"/>
-      <c r="BX23" s="45"/>
-      <c r="BY23" s="45"/>
-      <c r="BZ23" s="45"/>
-      <c r="CA23" s="45"/>
-      <c r="CB23" s="45"/>
-      <c r="CC23" s="45"/>
-      <c r="CD23" s="45"/>
-      <c r="CE23" s="45"/>
-      <c r="CF23" s="45"/>
-      <c r="CG23" s="45"/>
-      <c r="CH23" s="45"/>
-      <c r="CI23" s="45"/>
-      <c r="CJ23" s="45"/>
-      <c r="CK23" s="45"/>
-      <c r="CL23" s="45"/>
-      <c r="CM23" s="45"/>
-      <c r="CN23" s="45"/>
-      <c r="CO23" s="45"/>
-      <c r="CP23" s="45"/>
-      <c r="CQ23" s="45"/>
-      <c r="CR23" s="45"/>
-      <c r="CS23" s="45"/>
-      <c r="CT23" s="45"/>
-      <c r="CU23" s="45"/>
-      <c r="CV23" s="45"/>
-      <c r="CW23" s="45"/>
-      <c r="CX23" s="45"/>
-      <c r="CY23" s="45"/>
-      <c r="CZ23" s="45"/>
-      <c r="DA23" s="45"/>
-      <c r="DB23" s="45"/>
-      <c r="DC23" s="45"/>
-      <c r="DD23" s="45"/>
-      <c r="DE23" s="45"/>
-      <c r="DF23" s="45"/>
-      <c r="DG23" s="45"/>
-      <c r="DH23" s="45"/>
-      <c r="DI23" s="45"/>
-      <c r="DJ23" s="45"/>
-      <c r="DK23" s="45"/>
-      <c r="DL23" s="45"/>
-      <c r="DM23" s="45"/>
-      <c r="DN23" s="45"/>
-      <c r="DO23" s="45"/>
-      <c r="DP23" s="45"/>
-      <c r="DQ23" s="45"/>
-      <c r="DR23" s="45"/>
-      <c r="DS23" s="45"/>
-      <c r="DT23" s="45"/>
-      <c r="DU23" s="45"/>
-      <c r="DV23" s="45"/>
-      <c r="DW23" s="45"/>
-      <c r="DX23" s="45"/>
-      <c r="DY23" s="45"/>
-      <c r="DZ23" s="45"/>
-      <c r="EA23" s="45"/>
-      <c r="EB23" s="45"/>
-      <c r="EC23" s="45"/>
-      <c r="ED23" s="45"/>
-      <c r="EE23" s="45"/>
-      <c r="EF23" s="45"/>
-      <c r="EG23" s="45"/>
-      <c r="EH23" s="45"/>
-      <c r="EI23" s="45"/>
-      <c r="EJ23" s="45"/>
-      <c r="EK23" s="45"/>
-      <c r="EL23" s="45"/>
-      <c r="EM23" s="45"/>
-      <c r="EN23" s="45"/>
-      <c r="EO23" s="45"/>
-      <c r="EP23" s="45"/>
-      <c r="EQ23" s="45"/>
-      <c r="ER23" s="45"/>
-      <c r="ES23" s="45"/>
-      <c r="ET23" s="45"/>
-      <c r="EU23" s="45"/>
-      <c r="EV23" s="45"/>
-      <c r="EW23" s="45"/>
-      <c r="EX23" s="45"/>
-      <c r="EY23" s="45"/>
-      <c r="EZ23" s="45"/>
-      <c r="FA23" s="45"/>
-      <c r="FB23" s="45"/>
-      <c r="FC23" s="45"/>
-      <c r="FD23" s="45"/>
-      <c r="FE23" s="45"/>
-      <c r="FF23" s="45"/>
-      <c r="FG23" s="45"/>
-      <c r="FH23" s="45"/>
-      <c r="FI23" s="45"/>
-      <c r="FJ23" s="45"/>
-      <c r="FK23" s="45"/>
-      <c r="FL23" s="45"/>
-      <c r="FM23" s="45"/>
-      <c r="FN23" s="45"/>
-      <c r="FO23" s="45"/>
-      <c r="FP23" s="45"/>
-      <c r="FQ23" s="45"/>
-      <c r="FR23" s="45"/>
-      <c r="FS23" s="45"/>
-      <c r="FT23" s="45"/>
-      <c r="FU23" s="45"/>
-      <c r="FV23" s="45"/>
-      <c r="FW23" s="45"/>
-      <c r="FX23" s="45"/>
-      <c r="FY23" s="45"/>
-      <c r="FZ23" s="45"/>
-      <c r="GA23" s="45"/>
-      <c r="GB23" s="45"/>
-      <c r="GC23" s="45"/>
-      <c r="GD23" s="45"/>
-      <c r="GE23" s="45"/>
-      <c r="GF23" s="45"/>
-      <c r="GG23" s="45"/>
-      <c r="GH23" s="45"/>
-      <c r="GI23" s="45"/>
-      <c r="GJ23" s="45"/>
-      <c r="GK23" s="45"/>
-      <c r="GL23" s="45"/>
-      <c r="GM23" s="45"/>
-      <c r="GN23" s="45"/>
-      <c r="GO23" s="45"/>
-      <c r="GP23" s="45"/>
-      <c r="GQ23" s="45"/>
-      <c r="GR23" s="45"/>
-      <c r="GS23" s="45"/>
-      <c r="GT23" s="45"/>
-      <c r="GU23" s="45"/>
-      <c r="GV23" s="45"/>
-      <c r="GW23" s="45"/>
-      <c r="GX23" s="45"/>
-      <c r="GY23" s="45"/>
-      <c r="GZ23" s="45"/>
-      <c r="HA23" s="45"/>
-      <c r="HB23" s="45"/>
-      <c r="HC23" s="45"/>
-      <c r="HD23" s="45"/>
-      <c r="HE23" s="45"/>
-      <c r="HF23" s="45"/>
-      <c r="HG23" s="45"/>
-      <c r="HH23" s="45"/>
-      <c r="HI23" s="45"/>
-      <c r="HJ23" s="45"/>
-      <c r="HK23" s="45"/>
-      <c r="HL23" s="45"/>
-      <c r="HM23" s="45"/>
-      <c r="HN23" s="45"/>
-      <c r="HO23" s="45"/>
-      <c r="HP23" s="45"/>
-      <c r="HQ23" s="45"/>
-      <c r="HR23" s="45"/>
-      <c r="HS23" s="45"/>
-      <c r="HT23" s="45"/>
-      <c r="HU23" s="45"/>
-      <c r="HV23" s="45"/>
-      <c r="HW23" s="45"/>
-      <c r="HX23" s="45"/>
-      <c r="HY23" s="45"/>
-      <c r="HZ23" s="45"/>
-      <c r="IA23" s="45"/>
-      <c r="IB23" s="45"/>
-      <c r="IC23" s="45"/>
-      <c r="ID23" s="45"/>
-      <c r="IE23" s="45"/>
-      <c r="IF23" s="45"/>
-      <c r="IG23" s="45"/>
-      <c r="IH23" s="45"/>
-      <c r="II23" s="45"/>
-      <c r="IJ23" s="45"/>
-      <c r="IK23" s="45"/>
-      <c r="IL23" s="45"/>
-      <c r="IM23" s="45"/>
-      <c r="IN23" s="45"/>
-      <c r="IO23" s="45"/>
-      <c r="IP23" s="45"/>
-      <c r="IQ23" s="45"/>
-      <c r="IR23" s="45"/>
-      <c r="IS23" s="45"/>
-      <c r="IT23" s="45"/>
-      <c r="IU23" s="45"/>
-      <c r="IV23" s="45"/>
-      <c r="IW23" s="45"/>
-      <c r="IX23" s="45"/>
-      <c r="IY23" s="45"/>
-      <c r="IZ23" s="45"/>
-      <c r="JA23" s="45"/>
-      <c r="JB23" s="45"/>
-      <c r="JC23" s="45"/>
-      <c r="JD23" s="45"/>
-      <c r="JE23" s="45"/>
-      <c r="JF23" s="45"/>
-      <c r="JG23" s="45"/>
-      <c r="JH23" s="45"/>
-      <c r="JI23" s="45"/>
-      <c r="JJ23" s="45"/>
-      <c r="JK23" s="45"/>
-      <c r="JL23" s="45"/>
-      <c r="JM23" s="45"/>
-      <c r="JN23" s="45"/>
-      <c r="JO23" s="45"/>
-      <c r="JP23" s="45"/>
-      <c r="JQ23" s="45"/>
-      <c r="JR23" s="45"/>
-      <c r="JS23" s="45"/>
-      <c r="JT23" s="45"/>
-      <c r="JU23" s="45"/>
-      <c r="JV23" s="45"/>
-      <c r="JW23" s="45"/>
-      <c r="JX23" s="45"/>
-      <c r="JY23" s="45"/>
-      <c r="JZ23" s="45"/>
-      <c r="KA23" s="45"/>
-      <c r="KB23" s="45"/>
-      <c r="KC23" s="45"/>
-      <c r="KD23" s="45"/>
-      <c r="KE23" s="45"/>
-      <c r="KF23" s="45"/>
-      <c r="KG23" s="45"/>
-      <c r="KH23" s="45"/>
-      <c r="KI23" s="45"/>
-      <c r="KJ23" s="45"/>
-      <c r="KK23" s="45"/>
-      <c r="KL23" s="45"/>
-      <c r="KM23" s="45"/>
-      <c r="KN23" s="45"/>
-      <c r="KO23" s="45"/>
-      <c r="KP23" s="45"/>
-      <c r="KQ23" s="45"/>
-      <c r="KR23" s="45"/>
-      <c r="KS23" s="45"/>
-      <c r="KT23" s="45"/>
-      <c r="KU23" s="45"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="44"/>
+      <c r="Q23" s="44"/>
+      <c r="R23" s="44"/>
+      <c r="S23" s="44"/>
+      <c r="T23" s="44"/>
+      <c r="U23" s="44"/>
+      <c r="V23" s="44"/>
+      <c r="W23" s="44"/>
+      <c r="X23" s="44"/>
+      <c r="Y23" s="44"/>
+      <c r="Z23" s="44"/>
+      <c r="AA23" s="44"/>
+      <c r="AB23" s="44"/>
+      <c r="AC23" s="44"/>
+      <c r="AD23" s="44"/>
+      <c r="AE23" s="44"/>
+      <c r="AF23" s="44"/>
+      <c r="AG23" s="44"/>
+      <c r="AH23" s="44"/>
+      <c r="AI23" s="44"/>
+      <c r="AJ23" s="44"/>
+      <c r="AK23" s="44"/>
+      <c r="AL23" s="44"/>
+      <c r="AM23" s="44"/>
+      <c r="AN23" s="44"/>
+      <c r="AO23" s="44"/>
+      <c r="AP23" s="44"/>
+      <c r="AQ23" s="44"/>
+      <c r="AR23" s="44"/>
+      <c r="AS23" s="44"/>
+      <c r="AT23" s="44"/>
+      <c r="AU23" s="44"/>
+      <c r="AV23" s="44"/>
+      <c r="AW23" s="44"/>
+      <c r="AX23" s="44"/>
+      <c r="AY23" s="44"/>
+      <c r="AZ23" s="44"/>
+      <c r="BA23" s="44"/>
+      <c r="BB23" s="44"/>
+      <c r="BC23" s="44"/>
+      <c r="BD23" s="44"/>
+      <c r="BE23" s="44"/>
+      <c r="BF23" s="44"/>
+      <c r="BG23" s="44"/>
+      <c r="BH23" s="44"/>
+      <c r="BI23" s="44"/>
+      <c r="BJ23" s="44"/>
+      <c r="BK23" s="44"/>
+      <c r="BL23" s="44"/>
+      <c r="BM23" s="44"/>
+      <c r="BN23" s="44"/>
+      <c r="BO23" s="44"/>
+      <c r="BP23" s="44"/>
+      <c r="BQ23" s="44"/>
+      <c r="BR23" s="44"/>
+      <c r="BS23" s="44"/>
+      <c r="BT23" s="44"/>
+      <c r="BU23" s="44"/>
+      <c r="BV23" s="44"/>
+      <c r="BW23" s="44"/>
+      <c r="BX23" s="44"/>
+      <c r="BY23" s="44"/>
+      <c r="BZ23" s="44"/>
+      <c r="CA23" s="44"/>
+      <c r="CB23" s="44"/>
+      <c r="CC23" s="44"/>
+      <c r="CD23" s="44"/>
+      <c r="CE23" s="44"/>
+      <c r="CF23" s="44"/>
+      <c r="CG23" s="44"/>
+      <c r="CH23" s="44"/>
+      <c r="CI23" s="44"/>
+      <c r="CJ23" s="44"/>
+      <c r="CK23" s="44"/>
+      <c r="CL23" s="44"/>
+      <c r="CM23" s="44"/>
+      <c r="CN23" s="44"/>
+      <c r="CO23" s="44"/>
+      <c r="CP23" s="44"/>
+      <c r="CQ23" s="44"/>
+      <c r="CR23" s="44"/>
+      <c r="CS23" s="44"/>
+      <c r="CT23" s="44"/>
+      <c r="CU23" s="44"/>
+      <c r="CV23" s="44"/>
+      <c r="CW23" s="44"/>
+      <c r="CX23" s="44"/>
+      <c r="CY23" s="44"/>
+      <c r="CZ23" s="44"/>
+      <c r="DA23" s="44"/>
+      <c r="DB23" s="44"/>
+      <c r="DC23" s="44"/>
+      <c r="DD23" s="44"/>
+      <c r="DE23" s="44"/>
+      <c r="DF23" s="44"/>
+      <c r="DG23" s="44"/>
+      <c r="DH23" s="44"/>
+      <c r="DI23" s="44"/>
+      <c r="DJ23" s="44"/>
+      <c r="DK23" s="44"/>
+      <c r="DL23" s="44"/>
+      <c r="DM23" s="44"/>
+      <c r="DN23" s="44"/>
+      <c r="DO23" s="44"/>
+      <c r="DP23" s="44"/>
+      <c r="DQ23" s="44"/>
+      <c r="DR23" s="44"/>
+      <c r="DS23" s="44"/>
+      <c r="DT23" s="44"/>
+      <c r="DU23" s="44"/>
+      <c r="DV23" s="44"/>
+      <c r="DW23" s="44"/>
+      <c r="DX23" s="44"/>
+      <c r="DY23" s="44"/>
+      <c r="DZ23" s="44"/>
+      <c r="EA23" s="44"/>
+      <c r="EB23" s="44"/>
+      <c r="EC23" s="44"/>
+      <c r="ED23" s="44"/>
+      <c r="EE23" s="44"/>
+      <c r="EF23" s="44"/>
+      <c r="EG23" s="44"/>
+      <c r="EH23" s="44"/>
+      <c r="EI23" s="44"/>
+      <c r="EJ23" s="44"/>
+      <c r="EK23" s="44"/>
+      <c r="EL23" s="44"/>
+      <c r="EM23" s="44"/>
+      <c r="EN23" s="44"/>
+      <c r="EO23" s="44"/>
+      <c r="EP23" s="44"/>
+      <c r="EQ23" s="44"/>
+      <c r="ER23" s="44"/>
+      <c r="ES23" s="44"/>
+      <c r="ET23" s="44"/>
+      <c r="EU23" s="44"/>
+      <c r="EV23" s="44"/>
+      <c r="EW23" s="44"/>
+      <c r="EX23" s="44"/>
+      <c r="EY23" s="44"/>
+      <c r="EZ23" s="44"/>
+      <c r="FA23" s="44"/>
+      <c r="FB23" s="44"/>
+      <c r="FC23" s="44"/>
+      <c r="FD23" s="44"/>
+      <c r="FE23" s="44"/>
+      <c r="FF23" s="44"/>
+      <c r="FG23" s="44"/>
+      <c r="FH23" s="44"/>
+      <c r="FI23" s="44"/>
+      <c r="FJ23" s="44"/>
+      <c r="FK23" s="44"/>
+      <c r="FL23" s="44"/>
+      <c r="FM23" s="44"/>
+      <c r="FN23" s="44"/>
+      <c r="FO23" s="44"/>
+      <c r="FP23" s="44"/>
+      <c r="FQ23" s="44"/>
+      <c r="FR23" s="44"/>
+      <c r="FS23" s="44"/>
+      <c r="FT23" s="44"/>
+      <c r="FU23" s="44"/>
+      <c r="FV23" s="44"/>
+      <c r="FW23" s="44"/>
+      <c r="FX23" s="44"/>
+      <c r="FY23" s="44"/>
+      <c r="FZ23" s="44"/>
+      <c r="GA23" s="44"/>
+      <c r="GB23" s="44"/>
+      <c r="GC23" s="44"/>
+      <c r="GD23" s="44"/>
+      <c r="GE23" s="44"/>
+      <c r="GF23" s="44"/>
+      <c r="GG23" s="44"/>
+      <c r="GH23" s="44"/>
+      <c r="GI23" s="44"/>
+      <c r="GJ23" s="44"/>
+      <c r="GK23" s="44"/>
+      <c r="GL23" s="44"/>
+      <c r="GM23" s="44"/>
+      <c r="GN23" s="44"/>
+      <c r="GO23" s="44"/>
+      <c r="GP23" s="44"/>
+      <c r="GQ23" s="44"/>
+      <c r="GR23" s="44"/>
+      <c r="GS23" s="44"/>
+      <c r="GT23" s="44"/>
+      <c r="GU23" s="44"/>
+      <c r="GV23" s="44"/>
+      <c r="GW23" s="44"/>
+      <c r="GX23" s="44"/>
+      <c r="GY23" s="44"/>
+      <c r="GZ23" s="44"/>
+      <c r="HA23" s="44"/>
+      <c r="HB23" s="44"/>
+      <c r="HC23" s="44"/>
+      <c r="HD23" s="44"/>
+      <c r="HE23" s="44"/>
+      <c r="HF23" s="44"/>
+      <c r="HG23" s="44"/>
+      <c r="HH23" s="44"/>
+      <c r="HI23" s="44"/>
+      <c r="HJ23" s="44"/>
+      <c r="HK23" s="44"/>
+      <c r="HL23" s="44"/>
+      <c r="HM23" s="44"/>
+      <c r="HN23" s="44"/>
+      <c r="HO23" s="44"/>
+      <c r="HP23" s="44"/>
+      <c r="HQ23" s="44"/>
+      <c r="HR23" s="44"/>
+      <c r="HS23" s="44"/>
+      <c r="HT23" s="44"/>
+      <c r="HU23" s="44"/>
+      <c r="HV23" s="44"/>
+      <c r="HW23" s="44"/>
+      <c r="HX23" s="44"/>
+      <c r="HY23" s="44"/>
+      <c r="HZ23" s="44"/>
+      <c r="IA23" s="44"/>
+      <c r="IB23" s="44"/>
+      <c r="IC23" s="44"/>
+      <c r="ID23" s="44"/>
+      <c r="IE23" s="44"/>
+      <c r="IF23" s="44"/>
+      <c r="IG23" s="44"/>
+      <c r="IH23" s="44"/>
+      <c r="II23" s="44"/>
+      <c r="IJ23" s="44"/>
+      <c r="IK23" s="44"/>
+      <c r="IL23" s="44"/>
+      <c r="IM23" s="44"/>
+      <c r="IN23" s="44"/>
+      <c r="IO23" s="44"/>
+      <c r="IP23" s="44"/>
+      <c r="IQ23" s="44"/>
+      <c r="IR23" s="44"/>
+      <c r="IS23" s="44"/>
+      <c r="IT23" s="44"/>
+      <c r="IU23" s="44"/>
+      <c r="IV23" s="44"/>
+      <c r="IW23" s="44"/>
+      <c r="IX23" s="44"/>
+      <c r="IY23" s="44"/>
+      <c r="IZ23" s="44"/>
+      <c r="JA23" s="44"/>
+      <c r="JB23" s="44"/>
+      <c r="JC23" s="44"/>
+      <c r="JD23" s="44"/>
+      <c r="JE23" s="44"/>
+      <c r="JF23" s="44"/>
+      <c r="JG23" s="44"/>
+      <c r="JH23" s="44"/>
+      <c r="JI23" s="44"/>
+      <c r="JJ23" s="44"/>
+      <c r="JK23" s="44"/>
+      <c r="JL23" s="44"/>
+      <c r="JM23" s="44"/>
+      <c r="JN23" s="44"/>
+      <c r="JO23" s="44"/>
+      <c r="JP23" s="44"/>
+      <c r="JQ23" s="44"/>
+      <c r="JR23" s="44"/>
+      <c r="JS23" s="44"/>
+      <c r="JT23" s="44"/>
+      <c r="JU23" s="44"/>
+      <c r="JV23" s="44"/>
+      <c r="JW23" s="44"/>
+      <c r="JX23" s="44"/>
+      <c r="JY23" s="44"/>
+      <c r="JZ23" s="44"/>
+      <c r="KA23" s="44"/>
+      <c r="KB23" s="44"/>
+      <c r="KC23" s="44"/>
+      <c r="KD23" s="44"/>
+      <c r="KE23" s="44"/>
+      <c r="KF23" s="44"/>
+      <c r="KG23" s="44"/>
+      <c r="KH23" s="44"/>
+      <c r="KI23" s="44"/>
+      <c r="KJ23" s="44"/>
+      <c r="KK23" s="44"/>
+      <c r="KL23" s="44"/>
+      <c r="KM23" s="44"/>
+      <c r="KN23" s="44"/>
+      <c r="KO23" s="44"/>
+      <c r="KP23" s="44"/>
+      <c r="KQ23" s="44"/>
+      <c r="KR23" s="44"/>
+      <c r="KS23" s="44"/>
+      <c r="KT23" s="44"/>
+      <c r="KU23" s="44"/>
     </row>
     <row r="24" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="A24" s="38">
+      <c r="A24" s="37">
         <f>A23+0.1</f>
         <v>-0.9</v>
       </c>
-      <c r="B24" s="39">
+      <c r="B24" s="38">
         <f t="shared" ref="B24:B53" si="0">1-A24</f>
         <v>1.9</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="31"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="A25" s="38">
+      <c r="A25" s="37">
         <f t="shared" ref="A25:A32" si="1">A24+0.1</f>
         <v>-0.8</v>
       </c>
-      <c r="B25" s="39">
+      <c r="B25" s="38">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="31"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
     </row>
     <row r="26" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="A26" s="38">
+      <c r="A26" s="37">
         <f t="shared" si="1"/>
         <v>-0.70000000000000007</v>
       </c>
-      <c r="B26" s="39">
+      <c r="B26" s="38">
         <f t="shared" si="0"/>
         <v>1.7000000000000002</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="31"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
     </row>
     <row r="27" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="A27" s="38">
+      <c r="A27" s="37">
         <f t="shared" si="1"/>
         <v>-0.60000000000000009</v>
       </c>
-      <c r="B27" s="39">
+      <c r="B27" s="38">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="31"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
     </row>
     <row r="28" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="A28" s="38">
+      <c r="A28" s="37">
         <f t="shared" si="1"/>
         <v>-0.50000000000000011</v>
       </c>
-      <c r="B28" s="39">
+      <c r="B28" s="38">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="31"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
     </row>
     <row r="29" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="A29" s="38">
+      <c r="A29" s="37">
         <f t="shared" si="1"/>
         <v>-0.40000000000000013</v>
       </c>
-      <c r="B29" s="39">
+      <c r="B29" s="38">
         <f t="shared" si="0"/>
         <v>1.4000000000000001</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="31"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
     </row>
     <row r="30" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="A30" s="38">
+      <c r="A30" s="37">
         <f t="shared" si="1"/>
         <v>-0.30000000000000016</v>
       </c>
-      <c r="B30" s="39">
+      <c r="B30" s="38">
         <f t="shared" si="0"/>
         <v>1.3000000000000003</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="31"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
     </row>
     <row r="31" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="A31" s="38">
+      <c r="A31" s="37">
         <f t="shared" si="1"/>
         <v>-0.20000000000000015</v>
       </c>
-      <c r="B31" s="39">
+      <c r="B31" s="38">
         <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="31"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
     </row>
     <row r="32" spans="1:308" x14ac:dyDescent="0.2">
-      <c r="A32" s="38">
+      <c r="A32" s="37">
         <f t="shared" si="1"/>
         <v>-0.10000000000000014</v>
       </c>
-      <c r="B32" s="39">
+      <c r="B32" s="38">
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="31"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="38">
+      <c r="A33" s="37">
         <v>0</v>
       </c>
-      <c r="B33" s="39">
+      <c r="B33" s="38">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C33" s="30"/>
       <c r="D33" s="31"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="38">
+      <c r="A34" s="37">
         <f t="shared" ref="A34:A53" si="2">A33+0.1</f>
         <v>0.1</v>
       </c>
-      <c r="B34" s="39">
+      <c r="B34" s="38">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="38">
+      <c r="A35" s="37">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="B35" s="39">
+      <c r="B35" s="38">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="C35" s="30"/>
       <c r="D35" s="31"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="38">
+      <c r="A36" s="37">
         <f t="shared" si="2"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="B36" s="39">
+      <c r="B36" s="38">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="38">
+      <c r="A37" s="37">
         <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="B37" s="39">
+      <c r="B37" s="38">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="C37" s="30"/>
       <c r="D37" s="31"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="38">
+      <c r="A38" s="37">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="B38" s="39">
+      <c r="B38" s="38">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="31"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="38">
+      <c r="A39" s="37">
         <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="B39" s="39">
+      <c r="B39" s="38">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="31"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="38">
+      <c r="A40" s="37">
         <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
-      <c r="B40" s="39">
+      <c r="B40" s="38">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="C40" s="30"/>
       <c r="D40" s="31"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="38">
+      <c r="A41" s="37">
         <f t="shared" si="2"/>
         <v>0.79999999999999993</v>
       </c>
-      <c r="B41" s="39">
+      <c r="B41" s="38">
         <f t="shared" si="0"/>
         <v>0.20000000000000007</v>
       </c>
       <c r="C41" s="30"/>
       <c r="D41" s="31"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="38">
+      <c r="A42" s="37">
         <f t="shared" si="2"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="B42" s="39">
+      <c r="B42" s="38">
         <f t="shared" si="0"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="C42" s="30"/>
       <c r="D42" s="31"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="38">
+      <c r="A43" s="37">
         <f t="shared" si="2"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="B43" s="39">
+      <c r="B43" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C43" s="30"/>
       <c r="D43" s="31"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="38">
+      <c r="A44" s="37">
         <f t="shared" si="2"/>
         <v>1.0999999999999999</v>
       </c>
-      <c r="B44" s="39">
+      <c r="B44" s="38">
         <f t="shared" si="0"/>
         <v>-9.9999999999999867E-2</v>
       </c>
       <c r="C44" s="30"/>
       <c r="D44" s="31"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="38">
+      <c r="A45" s="37">
         <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
-      <c r="B45" s="39">
+      <c r="B45" s="38">
         <f t="shared" si="0"/>
         <v>-0.19999999999999996</v>
       </c>
       <c r="C45" s="30"/>
       <c r="D45" s="31"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="38">
+      <c r="A46" s="37">
         <f t="shared" si="2"/>
         <v>1.3</v>
       </c>
-      <c r="B46" s="39">
+      <c r="B46" s="38">
         <f t="shared" si="0"/>
         <v>-0.30000000000000004</v>
       </c>
       <c r="C46" s="30"/>
       <c r="D46" s="31"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="33"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="38">
+      <c r="A47" s="37">
         <f t="shared" si="2"/>
         <v>1.4000000000000001</v>
       </c>
-      <c r="B47" s="39">
+      <c r="B47" s="38">
         <f t="shared" si="0"/>
         <v>-0.40000000000000013</v>
       </c>
       <c r="C47" s="30"/>
       <c r="D47" s="31"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="38">
+      <c r="A48" s="37">
         <f t="shared" si="2"/>
         <v>1.5000000000000002</v>
       </c>
-      <c r="B48" s="39">
+      <c r="B48" s="38">
         <f t="shared" si="0"/>
         <v>-0.50000000000000022</v>
       </c>
       <c r="C48" s="30"/>
       <c r="D48" s="31"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="33"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="38">
+      <c r="A49" s="37">
         <f t="shared" si="2"/>
         <v>1.6000000000000003</v>
       </c>
-      <c r="B49" s="39">
+      <c r="B49" s="38">
         <f t="shared" si="0"/>
         <v>-0.60000000000000031</v>
       </c>
       <c r="C49" s="30"/>
       <c r="D49" s="31"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="33"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="38">
+      <c r="A50" s="37">
         <f t="shared" si="2"/>
         <v>1.7000000000000004</v>
       </c>
-      <c r="B50" s="39">
+      <c r="B50" s="38">
         <f t="shared" si="0"/>
         <v>-0.7000000000000004</v>
       </c>
       <c r="C50" s="30"/>
       <c r="D50" s="31"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="33"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="38">
+      <c r="A51" s="37">
         <f t="shared" si="2"/>
         <v>1.8000000000000005</v>
       </c>
-      <c r="B51" s="39">
+      <c r="B51" s="38">
         <f t="shared" si="0"/>
         <v>-0.80000000000000049</v>
       </c>
       <c r="C51" s="30"/>
       <c r="D51" s="31"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="33"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="38">
+      <c r="A52" s="37">
         <f t="shared" si="2"/>
         <v>1.9000000000000006</v>
       </c>
-      <c r="B52" s="39">
+      <c r="B52" s="38">
         <f t="shared" si="0"/>
         <v>-0.90000000000000058</v>
       </c>
       <c r="C52" s="30"/>
       <c r="D52" s="31"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="33"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="40">
+      <c r="A53" s="39">
         <f t="shared" si="2"/>
         <v>2.0000000000000004</v>
       </c>
-      <c r="B53" s="41">
+      <c r="B53" s="40">
         <f t="shared" si="0"/>
         <v>-1.0000000000000004</v>
       </c>
-      <c r="C53" s="34"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
-      <c r="H53" s="33"/>
-      <c r="I53" s="33"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="33"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F55" s="33"/>
-      <c r="G55" s="33"/>
-      <c r="H55" s="33"/>
-      <c r="I55" s="33"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B57" s="51" t="s">
+      <c r="B57" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="52"/>
+      <c r="C57" s="51"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B58" s="53"/>
-      <c r="C58" s="54"/>
+      <c r="B58" s="52"/>
+      <c r="C58" s="53"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B59" s="53"/>
-      <c r="C59" s="54"/>
+      <c r="B59" s="52"/>
+      <c r="C59" s="53"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B60" s="55"/>
-      <c r="C60" s="56"/>
+      <c r="B60" s="54"/>
+      <c r="C60" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>